<commit_message>
Subindo correção de documentos, logo e footer
</commit_message>
<xml_diff>
--- a/documentação/documentos/MATRIZ-RACI completo.xlsx
+++ b/documentação/documentos/MATRIZ-RACI completo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joyce Silva\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\prova_tudo\documentação\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,9 +16,6 @@
     <sheet name="Envolvovidos" sheetId="2" r:id="rId2"/>
     <sheet name="Descrição" sheetId="7" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="AgendaAno">#REF!</definedName>
     <definedName name="AgendaSemestre">#REF!</definedName>
@@ -34,12 +31,11 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Matriz Raci'!$4:$4</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="92">
   <si>
     <t>NOME</t>
   </si>
@@ -221,21 +217,6 @@
     <t>William Bezerra</t>
   </si>
   <si>
-    <t>Igor Rodrigues</t>
-  </si>
-  <si>
-    <t>Ellias</t>
-  </si>
-  <si>
-    <t>Rodolfo</t>
-  </si>
-  <si>
-    <t>Alexandre</t>
-  </si>
-  <si>
-    <t>Charlles Sousa</t>
-  </si>
-  <si>
     <t>Joyce Silva</t>
   </si>
   <si>
@@ -308,12 +289,6 @@
     <t>paginação</t>
   </si>
   <si>
-    <t>Luzia</t>
-  </si>
-  <si>
-    <t>Coordenador do NPI</t>
-  </si>
-  <si>
     <t>Rogério</t>
   </si>
   <si>
@@ -324,6 +299,18 @@
   </si>
   <si>
     <t>1.23</t>
+  </si>
+  <si>
+    <t>Eduardo Ferreira</t>
+  </si>
+  <si>
+    <t>Yves Guilherme</t>
+  </si>
+  <si>
+    <t>Akira</t>
+  </si>
+  <si>
+    <t>Igor Jesus</t>
   </si>
 </sst>
 </file>
@@ -492,7 +479,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -532,9 +519,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -555,10 +539,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="h:mm;@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="h:mm;@"/>
     </dxf>
     <dxf>
       <fill>
@@ -1760,23 +1744,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Matriz Raci"/>
-      <sheetName val="Envolvovidos"/>
-      <sheetName val="Descrição"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tabListadeAulas" displayName="tabListadeAulas" ref="B4:H27" totalsRowShown="0">
   <tableColumns count="7">
@@ -1786,7 +1753,7 @@
     <tableColumn id="4" name="Responsável (Responsible)"/>
     <tableColumn id="5" name="Aprovar (Accountable )"/>
     <tableColumn id="6" name="Consultado (Consulted)"/>
-    <tableColumn id="7" name="Informado (Informed)" dataDxfId="1"/>
+    <tableColumn id="7" name="Informado (Informed)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Visão geral do semestre" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1798,10 +1765,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tabTrabalho" displayName="tabTrabalho" ref="B4:C20" totalsRowShown="0">
-  <autoFilter ref="B4:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="tabTrabalho" displayName="tabTrabalho" ref="B4:C18" totalsRowShown="0">
+  <autoFilter ref="B4:C18"/>
   <tableColumns count="2">
-    <tableColumn id="6" name="NOME" dataDxfId="2">
+    <tableColumn id="6" name="NOME" dataDxfId="1">
       <calculatedColumnFormula>VLOOKUP(#REF!,tabListadeAulas[],2,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" name="FUNÇÃO" dataDxfId="0"/>
@@ -2087,8 +2054,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2147,16 +2114,16 @@
         <v>58</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2170,16 +2137,16 @@
         <v>32</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2190,19 +2157,19 @@
         <v>35</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2210,22 +2177,22 @@
         <v>10</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2236,19 +2203,19 @@
         <v>31</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2262,16 +2229,16 @@
         <v>38</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
@@ -2284,19 +2251,19 @@
         <v>31</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2310,16 +2277,16 @@
         <v>49</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2330,19 +2297,19 @@
         <v>31</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2353,19 +2320,19 @@
         <v>31</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2373,22 +2340,22 @@
         <v>45</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2399,19 +2366,19 @@
         <v>35</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2425,16 +2392,16 @@
         <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2451,13 +2418,13 @@
         <v>59</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2471,16 +2438,16 @@
         <v>44</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2491,42 +2458,42 @@
         <v>35</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2540,16 +2507,16 @@
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2557,22 +2524,22 @@
         <v>55</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2583,19 +2550,19 @@
         <v>31</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2609,62 +2576,62 @@
         <v>41</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="5" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2683,7 +2650,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Envolvovidos!$B$5:$B$27</xm:f>
+            <xm:f>Envolvovidos!$B$5:$B$25</xm:f>
           </x14:formula1>
           <xm:sqref>E5:H27</xm:sqref>
         </x14:dataValidation>
@@ -2699,9 +2666,11 @@
     <tabColor theme="4" tint="-0.249977111117893"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:C20"/>
+  <dimension ref="B1:C18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2732,88 +2701,72 @@
         <v>0</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="C13" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>90</v>
-      </c>
+    <row r="11" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
     </row>
     <row r="15" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13"/>
@@ -2830,14 +2783,6 @@
     <row r="18" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="13"/>
       <c r="C18" s="14"/>
-    </row>
-    <row r="19" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-    </row>
-    <row r="20" spans="2:3" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>